<commit_message>
vault backup: 2023-08-19 00:05:59
</commit_message>
<xml_diff>
--- a/Space Routing/survey.xlsx
+++ b/Space Routing/survey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Obsidian\Space Routing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\obsidian\Space Routing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{802D0DB1-E96B-4D73-9E6E-59F0D3EEAA01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A8FFBA-AAC5-40D0-A122-4AED26B7DC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17580" xr2:uid="{DF096129-A6C5-4068-AD2B-234CDF438231}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{DF096129-A6C5-4068-AD2B-234CDF438231}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,61 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>publication</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Advantage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shortcoming</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TMC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multipath Cooperative Routing with Efficient Acknowledgement for LEO Satellite Networks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 减少ACK排队对数据传输的影响
+2.多径提高系统的吞度量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1.多径路由+网络编码
+2. challenge:由于卫星链路的传播时延长，ACK的停等机制和hop-by-hop的ACK机制造成了长的时延
+3.多径选路：定时发送probe，然后在终点选取n条不相交的传输路径，然后传输给源节点
+4.网络编码：把多个数据包线性编码为一个batch
+5.NO-wait-ACK: 发送完当前batch后持续发送下一个batch,无需等待ACK，如果发送过的batch超时未收到ACK则重传
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.选路策略的overhead过大
+2. 仅采用线性的网络编码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -39,6 +91,22 @@
       <sz val="9"/>
       <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -65,9 +133,27 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -383,15 +469,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{630CE233-CC1B-4224-A6EB-3B97038C47EC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="45.4140625" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" customWidth="1"/>
+    <col min="4" max="4" width="47.4140625" customWidth="1"/>
+    <col min="5" max="5" width="59.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="159.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
vault backup: 2023-08-25 22:26:25
</commit_message>
<xml_diff>
--- a/Space Routing/survey.xlsx
+++ b/Space Routing/survey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\obsidian\Space Routing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C6FD0D-C45A-439C-A995-50237CE1D607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B351A4E-03BB-4E40-8115-AC93E91BA1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{DF096129-A6C5-4068-AD2B-234CDF438231}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="28800" windowHeight="15370" xr2:uid="{DF096129-A6C5-4068-AD2B-234CDF438231}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -97,6 +97,19 @@
     <t>1.信号灯算法考虑了附近的卫星状态
 2.提出ISL在极地地区会与相邻轨道的卫星断开连接，这个结论有点验证，目前我没有查到其他资料这么说
 3.提出公共缓存队列来存储没有下一跳的数据包，减少数据的丢包率。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Analysis of Inter-Satellite Link Paths for LEO Mega-Constellation Networks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TVT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.提出通过经纬度计算估算两个卫星之间的ISL跳数，其实可以通过给卫星编号来计算。。。。
+2.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -498,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{630CE233-CC1B-4224-A6EB-3B97038C47EC}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -564,6 +577,17 @@
         <v>13</v>
       </c>
     </row>
+    <row r="4" spans="1:5" ht="112.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
vault backup: 2023-08-26 22:59:46
</commit_message>
<xml_diff>
--- a/Space Routing/survey.xlsx
+++ b/Space Routing/survey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\obsidian\Space Routing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B351A4E-03BB-4E40-8115-AC93E91BA1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05F81C1-3058-4CF9-958F-60F07B8ADDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="28800" windowHeight="15370" xr2:uid="{DF096129-A6C5-4068-AD2B-234CDF438231}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{DF096129-A6C5-4068-AD2B-234CDF438231}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -109,7 +109,17 @@
   </si>
   <si>
     <t>1.提出通过经纬度计算估算两个卫星之间的ISL跳数，其实可以通过给卫星编号来计算。。。。
-2.</t>
+2.统计了ISL跳数分布的规律</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.计算跳数的算法太复杂但是没有意义。。。。
+2.仅研究了跳数分布的规律。。。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.在目前的卫星部署模式下（每个轨道卫星的数量大于轨道的跳数），那么横向传输的跳数少于纵向传播的跳数；路由策略可优先考虑横向传播。
+2.卫星相对于赤道的偏移量越大，跳数越少</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -514,19 +524,19 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="45.4140625" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" customWidth="1"/>
-    <col min="4" max="4" width="47.4140625" customWidth="1"/>
-    <col min="5" max="5" width="59.1640625" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.640625" customWidth="1"/>
+    <col min="4" max="4" width="47.42578125" customWidth="1"/>
+    <col min="5" max="5" width="59.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="22.75" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -543,7 +553,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="159.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="159.55000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -560,7 +570,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="132" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="132" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -577,7 +587,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="112.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="112.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -586,6 +596,12 @@
       </c>
       <c r="C4" s="6" t="s">
         <v>17</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2023-09-01 22:04:18
</commit_message>
<xml_diff>
--- a/Space Routing/survey.xlsx
+++ b/Space Routing/survey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\obsidian\Space Routing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leo/obsidian/Space Routing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05F81C1-3058-4CF9-958F-60F07B8ADDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6531B40-A800-A741-AEFE-85645B0E52B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{DF096129-A6C5-4068-AD2B-234CDF438231}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18000" xr2:uid="{DF096129-A6C5-4068-AD2B-234CDF438231}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -122,12 +122,57 @@
 2.卫星相对于赤道的偏移量越大，跳数越少</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Compact explicit multi-path routing for LEO satellite networks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HPSR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.对路径进行编码，用全局的编码替代header里面的路径，以此减少传输的消耗。
+2.如果路径编码无效，则使用默认最短路径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.指出ISL由于天线转向等因素在纬度70度左右会断开连接，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.过于简单，只是减少了header的大小，减少的传输消耗的效果有待商榷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Computer Networks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Distributed on-demand routing for LEO satellite systems</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.提出收缩广播的区域，在小范围内通过广播寻找最短路径。
+2.寻路方式：通过广播探测包寻找最短路径，每条路径有一定的有效期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.同样指出ISL在极低附近会断开与相邻轨道的连接
+2.缩小广播范围确实能减少寻路开销</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.广播域限缩在源/目的节点内的矩形内，当长距离传输时，广播域会非常大，
+2.考虑到排队时延，局部网络拥塞可能导致广播域内找不到时延低的路径
+3.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -521,22 +566,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{630CE233-CC1B-4224-A6EB-3B97038C47EC}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="45.640625" customWidth="1"/>
-    <col min="4" max="4" width="47.42578125" customWidth="1"/>
-    <col min="5" max="5" width="59.140625" customWidth="1"/>
+    <col min="1" max="1" width="45.5" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.6640625" customWidth="1"/>
+    <col min="4" max="4" width="47.5" customWidth="1"/>
+    <col min="5" max="5" width="59.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="22.75" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="23">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -553,7 +598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="159.55000000000001" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="159.5" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -570,7 +615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="132" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="132" customHeight="1">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -587,7 +632,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="112.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="112.5" customHeight="1">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -602,6 +647,40 @@
       </c>
       <c r="E4" s="6" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="100" customHeight="1">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="92" customHeight="1">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2023-09-06 17:02:24
</commit_message>
<xml_diff>
--- a/Space Routing/survey.xlsx
+++ b/Space Routing/survey.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leo/obsidian/Space Routing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\obsidian\Space Routing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6531B40-A800-A741-AEFE-85645B0E52B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6DBA4E-67DD-48C0-B5D1-34637B32553F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18000" xr2:uid="{DF096129-A6C5-4068-AD2B-234CDF438231}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{DF096129-A6C5-4068-AD2B-234CDF438231}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -162,9 +162,9 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.广播域限缩在源/目的节点内的矩形内，当长距离传输时，广播域会非常大，
+    <t xml:space="preserve">1.广播域限缩在源/目的节点内的矩形内，当长距离传输时，广播域会非常大，
 2.考虑到排队时延，局部网络拥塞可能导致广播域内找不到时延低的路径
-3.</t>
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -172,7 +172,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -568,20 +568,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{630CE233-CC1B-4224-A6EB-3B97038C47EC}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="45.5" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.640625" customWidth="1"/>
     <col min="4" max="4" width="47.5" customWidth="1"/>
-    <col min="5" max="5" width="59.1640625" customWidth="1"/>
+    <col min="5" max="5" width="59.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23">
+    <row r="1" spans="1:5" ht="22.75" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -598,7 +598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="159.5" customHeight="1">
+    <row r="2" spans="1:5" ht="159.55000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -615,7 +615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="132" customHeight="1">
+    <row r="3" spans="1:5" ht="132" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -632,7 +632,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="112.5" customHeight="1">
+    <row r="4" spans="1:5" ht="112.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -649,7 +649,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="100" customHeight="1">
+    <row r="5" spans="1:5" ht="100" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -666,7 +666,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="92" customHeight="1">
+    <row r="6" spans="1:5" ht="92.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
vault backup: 2023-09-11 09:10:26
</commit_message>
<xml_diff>
--- a/Space Routing/survey.xlsx
+++ b/Space Routing/survey.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leo/obsidian/Space Routing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Obsidian\Space Routing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6531B40-A800-A741-AEFE-85645B0E52B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA5F9DB-E9BD-4F16-81FE-CE554DF00CCF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18000" xr2:uid="{DF096129-A6C5-4068-AD2B-234CDF438231}"/>
   </bookViews>
@@ -172,7 +172,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -568,11 +568,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{630CE233-CC1B-4224-A6EB-3B97038C47EC}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45.5" customWidth="1"/>
     <col min="2" max="2" width="24.1640625" style="1" customWidth="1"/>
@@ -581,7 +581,7 @@
     <col min="5" max="5" width="59.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23">
+    <row r="1" spans="1:5" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -598,7 +598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="159.5" customHeight="1">
+    <row r="2" spans="1:5" ht="159.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -615,7 +615,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="132" customHeight="1">
+    <row r="3" spans="1:5" ht="132" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -632,7 +632,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="112.5" customHeight="1">
+    <row r="4" spans="1:5" ht="112.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -649,7 +649,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="100" customHeight="1">
+    <row r="5" spans="1:5" ht="100" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -666,7 +666,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="92" customHeight="1">
+    <row r="6" spans="1:5" ht="92" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>

</xml_diff>